<commit_message>
versão de download dos documentos allianz
</commit_message>
<xml_diff>
--- a/dados/processos_2.xlsx
+++ b/dados/processos_2.xlsx
@@ -1,35 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitor\Documents\Repositórios\automação\ressarcimento\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8535D132-0ABC-4822-B2B2-75E4999D105E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65431205-8860-482C-8D5C-19694943A540}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="11385" xr2:uid="{BFC620C7-56B0-4F6C-96EB-D5FF41980CED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -43,13 +29,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,7 +52,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -72,14 +71,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -92,7 +97,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -126,20 +131,20 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -167,31 +172,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -219,23 +207,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -247,171 +218,194 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A875AD2-E810-4A66-BF53-D48990E69547}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>16339902</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>16247971</v>
+    <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>16129616</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>